<commit_message>
Restrict distributions to the ones in the lectures
</commit_message>
<xml_diff>
--- a/tramDrivingTimes_distributionAnalysis.xlsx
+++ b/tramDrivingTimes_distributionAnalysis.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="3" r:id="rId1"/>
     <sheet name="Distribution Fit" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Overview!$A$1:$C$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Overview!$A$1:$C$7</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="64">
   <si>
     <t>Graadt van Roggenweg</t>
   </si>
@@ -89,36 +89,6 @@
     <t>Average rank</t>
   </si>
   <si>
-    <t>Gen. Extreme Value</t>
-  </si>
-  <si>
-    <t>Dagum (4P)</t>
-  </si>
-  <si>
-    <t>Pearson 6 (4P)</t>
-  </si>
-  <si>
-    <t>Log-Logistic (3P)</t>
-  </si>
-  <si>
-    <t>Burr (4P)</t>
-  </si>
-  <si>
-    <t>Dagum</t>
-  </si>
-  <si>
-    <t>Burr</t>
-  </si>
-  <si>
-    <t>Cauchy</t>
-  </si>
-  <si>
-    <t>Hypersecant</t>
-  </si>
-  <si>
-    <t>a=205,52, b=420,17, g=-370,8</t>
-  </si>
-  <si>
     <t>Occurrences</t>
   </si>
   <si>
@@ -131,31 +101,125 @@
     <t>Red is a bad rank, green is a good rank.</t>
   </si>
   <si>
-    <t>The two most occurring and best ranked distributions seem to be Burr (4P) and Log-Logistic (3P).</t>
-  </si>
-  <si>
-    <t>s=5,6634, m=82,179</t>
-  </si>
-  <si>
-    <t>s=2,7435, m=73,803</t>
-  </si>
-  <si>
-    <t>s=4,7494, m=98,213</t>
-  </si>
-  <si>
-    <t>s=3,3523, m=93,207</t>
-  </si>
-  <si>
-    <t>s=5,8397, m=146,2</t>
-  </si>
-  <si>
-    <t>s=3,2803, m=82,154</t>
+    <t>Exponential</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>Lognormal</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Uniform</t>
+  </si>
+  <si>
+    <t>Weibull</t>
+  </si>
+  <si>
+    <t>a=16.924, b=4.1458</t>
+  </si>
+  <si>
+    <t>a=6.2438, b=75.265</t>
+  </si>
+  <si>
+    <t>s=0.19242, m=4.2303</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>s=11,901, m=125.64</t>
+  </si>
+  <si>
+    <t>s=0.08708, m=4.8295</t>
+  </si>
+  <si>
+    <t>a=111.46, b=1.1273</t>
+  </si>
+  <si>
+    <t>s=4.1886, m=48.381</t>
+  </si>
+  <si>
+    <t>s=0.09119, m=3.8957</t>
+  </si>
+  <si>
+    <t>a=138.99, b=0.35529</t>
+  </si>
+  <si>
+    <t>a=130.26, b=0.66987</t>
+  </si>
+  <si>
+    <t>s=7.6455, m=87.261</t>
+  </si>
+  <si>
+    <t>s=0.0934, m=4.4649</t>
+  </si>
+  <si>
+    <t>s=0.08686, m=4.3869</t>
+  </si>
+  <si>
+    <t>a=105.27, b=0.76678</t>
+  </si>
+  <si>
+    <t>s=7.8773, m=80.719</t>
+  </si>
+  <si>
+    <t>a=21.989, b=3.8647</t>
+  </si>
+  <si>
+    <t>s=0.14103, m=4.4296</t>
+  </si>
+  <si>
+    <t>s=18.123, m=84.982</t>
+  </si>
+  <si>
+    <t>The most occurring and best ranked distribution seems to be Lognormal.</t>
+  </si>
+  <si>
+    <t>s=0.30879, m=4.443</t>
+  </si>
+  <si>
+    <t>s=0.07068, m=4.1508</t>
+  </si>
+  <si>
+    <t>s=0.07611, m=4.2966</t>
+  </si>
+  <si>
+    <t>s=0.10661, m=4.3177</t>
+  </si>
+  <si>
+    <t>s=0.22735, m=4.6524</t>
+  </si>
+  <si>
+    <t>s=0.08685, m=4.0343</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>s/m</t>
+  </si>
+  <si>
+    <t>Standard deviation and mean for the Lognormal fitted distributions.</t>
+  </si>
+  <si>
+    <t>The standard deviation is on average 3,01% of the mean.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="171" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -210,11 +274,20 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -223,11 +296,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -250,6 +320,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
@@ -545,165 +627,324 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1">
+      <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="11" t="s">
+      <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="8">
+        <f>COUNTIF('Distribution Fit'!B:B, Overview!A2)</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
+        <f>IFERROR(SUMIF('Distribution Fit'!B:B, Overview!A2, 'Distribution Fit'!J:J) / B2, 6)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="8">
+        <f>COUNTIF('Distribution Fit'!B:B, Overview!A3)</f>
+        <v>13</v>
+      </c>
+      <c r="C3" s="6">
+        <f>SUMIF('Distribution Fit'!B:B, Overview!A3, 'Distribution Fit'!J:J) / B3</f>
+        <v>2.1282051282051282</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="9">
-        <f>COUNTIF('Distribution Fit'!B:B, Overview!A2)</f>
-        <v>4</v>
-      </c>
-      <c r="C2" s="7">
-        <f>SUMIF('Distribution Fit'!B:B, Overview!A2, 'Distribution Fit'!J:J) / B2</f>
-        <v>4.333333333333333</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="9">
-        <f>COUNTIF('Distribution Fit'!B:B, Overview!A3)</f>
-        <v>7</v>
-      </c>
-      <c r="C3" s="7">
-        <f>SUMIF('Distribution Fit'!B:B, Overview!A3, 'Distribution Fit'!J:J) / B3</f>
-        <v>2.2380952380952377</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="11" t="s">
+      <c r="B4" s="8">
+        <f>COUNTIF('Distribution Fit'!B:B, Overview!A4)</f>
+        <v>12</v>
+      </c>
+      <c r="C4" s="6">
+        <f>SUMIF('Distribution Fit'!B:B, Overview!A4, 'Distribution Fit'!J:J) / B4</f>
+        <v>1.5833333333333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="9">
-        <f>COUNTIF('Distribution Fit'!B:B, Overview!A4)</f>
-        <v>6</v>
-      </c>
-      <c r="C4" s="7">
-        <f>SUMIF('Distribution Fit'!B:B, Overview!A4, 'Distribution Fit'!J:J) / B4</f>
-        <v>2.9444444444444442</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <f>COUNTIF('Distribution Fit'!B:B, Overview!A5)</f>
-        <v>5</v>
-      </c>
-      <c r="C5" s="7">
+        <v>13</v>
+      </c>
+      <c r="C5" s="6">
         <f>SUMIF('Distribution Fit'!B:B, Overview!A5, 'Distribution Fit'!J:J) / B5</f>
-        <v>4.333333333333333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="9">
+        <v>2.2051282051282053</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="8">
         <f>COUNTIF('Distribution Fit'!B:B, Overview!A6)</f>
-        <v>3</v>
-      </c>
-      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6">
         <f>SUMIF('Distribution Fit'!B:B, Overview!A6, 'Distribution Fit'!J:J) / B6</f>
-        <v>2.8888888888888888</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="8">
         <f>COUNTIF('Distribution Fit'!B:B, Overview!A7)</f>
-        <v>4</v>
-      </c>
-      <c r="C7" s="7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="6">
         <f>SUMIF('Distribution Fit'!B:B, Overview!A7, 'Distribution Fit'!J:J) / B7</f>
-        <v>8.6666666666666661</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="9">
-        <f>COUNTIF('Distribution Fit'!B:B, Overview!A8)</f>
-        <v>1</v>
-      </c>
-      <c r="C8" s="7">
-        <f>SUMIF('Distribution Fit'!B:B, Overview!A8, 'Distribution Fit'!J:J) / B8</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="11" t="s">
+        <v>2.4444444444444446</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="9">
-        <f>COUNTIF('Distribution Fit'!B:B, Overview!A9)</f>
-        <v>11</v>
-      </c>
-      <c r="C9" s="7">
-        <f>SUMIF('Distribution Fit'!B:B, Overview!A9, 'Distribution Fit'!J:J) / B9</f>
-        <v>2.939393939393939</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="9">
-        <f>COUNTIF('Distribution Fit'!B:B, Overview!A10)</f>
-        <v>1</v>
-      </c>
-      <c r="C10" s="7">
-        <f>SUMIF('Distribution Fit'!B:B, Overview!A10, 'Distribution Fit'!J:J) / B10</f>
-        <v>8.6666666666666661</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="B11" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="11" t="s">
-        <v>37</v>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="18">
+        <v>0.19242000000000001</v>
+      </c>
+      <c r="B14" s="17">
+        <v>4.2302999999999997</v>
+      </c>
+      <c r="C14" s="17">
+        <f>A14/B14</f>
+        <v>4.5486135735054258E-2</v>
+      </c>
+      <c r="D14" s="14"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="18">
+        <v>8.7080000000000005E-2</v>
+      </c>
+      <c r="B15" s="17">
+        <v>4.8295000000000003</v>
+      </c>
+      <c r="C15" s="17">
+        <f t="shared" ref="C15:C26" si="0">A15/B15</f>
+        <v>1.8030852055078164E-2</v>
+      </c>
+      <c r="D15" s="14"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="18">
+        <v>9.1189999999999993E-2</v>
+      </c>
+      <c r="B16" s="17">
+        <v>3.8957000000000002</v>
+      </c>
+      <c r="C16" s="17">
+        <f t="shared" si="0"/>
+        <v>2.3407859948147956E-2</v>
+      </c>
+      <c r="D16" s="14"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="18">
+        <v>9.3399999999999997E-2</v>
+      </c>
+      <c r="B17" s="17">
+        <v>4.4649000000000001</v>
+      </c>
+      <c r="C17" s="17">
+        <f t="shared" si="0"/>
+        <v>2.0918721583910053E-2</v>
+      </c>
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="18">
+        <v>8.6860000000000007E-2</v>
+      </c>
+      <c r="B18" s="17">
+        <v>4.3868999999999998</v>
+      </c>
+      <c r="C18" s="17">
+        <f t="shared" si="0"/>
+        <v>1.979985867013153E-2</v>
+      </c>
+      <c r="D18" s="14"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="18">
+        <v>0.14102999999999999</v>
+      </c>
+      <c r="B19" s="17">
+        <v>4.4295999999999998</v>
+      </c>
+      <c r="C19" s="17">
+        <f t="shared" si="0"/>
+        <v>3.1838089217988079E-2</v>
+      </c>
+      <c r="D19" s="14"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="18">
+        <v>8.6849999999999997E-2</v>
+      </c>
+      <c r="B20" s="17">
+        <v>4.0343</v>
+      </c>
+      <c r="C20" s="17">
+        <f t="shared" si="0"/>
+        <v>2.15278982723149E-2</v>
+      </c>
+      <c r="D20" s="14"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="18">
+        <v>0.22735</v>
+      </c>
+      <c r="B21" s="17">
+        <v>4.6524000000000001</v>
+      </c>
+      <c r="C21" s="17">
+        <f t="shared" si="0"/>
+        <v>4.886725131115123E-2</v>
+      </c>
+      <c r="D21" s="14"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="18">
+        <v>0.10661</v>
+      </c>
+      <c r="B22" s="17">
+        <v>4.3177000000000003</v>
+      </c>
+      <c r="C22" s="17">
+        <f t="shared" si="0"/>
+        <v>2.4691386617875254E-2</v>
+      </c>
+      <c r="D22" s="14"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="18">
+        <v>7.6109999999999997E-2</v>
+      </c>
+      <c r="B23" s="17">
+        <v>4.2965999999999998</v>
+      </c>
+      <c r="C23" s="17">
+        <f t="shared" si="0"/>
+        <v>1.7714006423683842E-2</v>
+      </c>
+      <c r="D23" s="14"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="18">
+        <v>7.0680000000000007E-2</v>
+      </c>
+      <c r="B24" s="17">
+        <v>4.1508000000000003</v>
+      </c>
+      <c r="C24" s="17">
+        <f t="shared" si="0"/>
+        <v>1.7028042786932641E-2</v>
+      </c>
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="18">
+        <v>0.30879000000000001</v>
+      </c>
+      <c r="B25" s="17">
+        <v>4.4429999999999996</v>
+      </c>
+      <c r="C25" s="17">
+        <f t="shared" si="0"/>
+        <v>6.950033760972317E-2</v>
+      </c>
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26" spans="1:4" s="22" customFormat="1">
+      <c r="A26" s="19">
+        <f>AVERAGE(A14:A25)</f>
+        <v>0.13069750000000002</v>
+      </c>
+      <c r="B26" s="20">
+        <f>AVERAGE(B14:B25)</f>
+        <v>4.3443083333333332</v>
+      </c>
+      <c r="C26" s="20">
+        <f t="shared" si="0"/>
+        <v>3.008476608282485E-2</v>
+      </c>
+      <c r="D26" s="21"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="16"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="14"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="10" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:J13">
     <sortCondition ref="A2:A13"/>
   </sortState>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="B1:B12 B27:B1048576">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -715,7 +956,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C1:C12 C27:C1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -728,6 +969,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -735,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -753,66 +995,78 @@
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="13"/>
+      <c r="H1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="13"/>
+      <c r="J1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1">
-      <c r="D2" s="3" t="s">
+    <row r="2" spans="1:10" s="2" customFormat="1">
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="4" customFormat="1">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:10" s="3" customFormat="1">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>6.3630000000000006E-2</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
+      <c r="F4">
+        <v>10.618</v>
+      </c>
       <c r="G4">
         <v>1</v>
+      </c>
+      <c r="H4">
+        <v>117.7</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -824,288 +1078,405 @@
     </row>
     <row r="5" spans="1:10">
       <c r="B5" t="s">
-        <v>24</v>
+        <v>32</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5">
+        <v>0.10729</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
+      <c r="F5">
+        <v>54.533999999999999</v>
+      </c>
       <c r="G5">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>2.6666666666666665</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="B6" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6">
+        <v>0.12994</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
+      <c r="F6">
+        <v>38.067999999999998</v>
+      </c>
       <c r="G6">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>305.39</v>
       </c>
       <c r="I6">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>8.6666666666666661</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="4" customFormat="1">
-      <c r="A7" s="4" t="s">
+        <v>2.3333333333333335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="3" customFormat="1">
+      <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="B8" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="D8">
-        <v>3.1710000000000002E-2</v>
+        <v>9.0279999999999999E-2</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>1.5441</v>
+        <v>20.172000000000001</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>39.165999999999997</v>
+        <v>129.74</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>1.6666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" t="s">
         <v>28</v>
       </c>
+      <c r="C9" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="D9">
-        <v>3.2759999999999997E-2</v>
+        <v>0.10631</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9">
-        <v>2.0714000000000001</v>
+        <v>28.437999999999999</v>
       </c>
       <c r="G9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H9">
-        <v>43.935000000000002</v>
+        <v>194.24</v>
       </c>
       <c r="I9">
         <v>3</v>
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2.3333333333333335</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="B10" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D10">
-        <v>3.2930000000000001E-2</v>
+        <v>0.11645999999999999</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
       <c r="F10">
-        <v>1.5335000000000001</v>
+        <v>36.731000000000002</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H10">
-        <v>79.754000000000005</v>
+        <v>172.8</v>
       </c>
       <c r="I10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J10">
         <f t="shared" si="0"/>
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="4" customFormat="1">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:10" s="3" customFormat="1">
+      <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="B12" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12">
+        <v>0.11527999999999999</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
+      <c r="F12">
+        <v>23.617000000000001</v>
+      </c>
       <c r="G12">
         <v>1</v>
       </c>
+      <c r="H12">
+        <v>177.51</v>
+      </c>
       <c r="I12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="D13">
-        <v>8.0390000000000003E-2</v>
+        <v>0.12222</v>
       </c>
       <c r="E13">
         <v>2</v>
       </c>
       <c r="F13">
-        <v>6.6883999999999997</v>
+        <v>24.041</v>
       </c>
       <c r="G13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>58.929000000000002</v>
+        <v>172.16</v>
       </c>
       <c r="I13">
         <v>2</v>
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="B14" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14">
+        <v>0.13585</v>
       </c>
       <c r="E14">
         <v>3</v>
       </c>
+      <c r="F14">
+        <v>33.000999999999998</v>
+      </c>
       <c r="G14">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>172.16</v>
       </c>
       <c r="I14">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>6.333333333333333</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="4" customFormat="1">
-      <c r="A15" s="4" t="s">
+        <v>2.3333333333333335</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="3" customFormat="1">
+      <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16">
+        <v>9.0079999999999993E-2</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
+      <c r="F16">
+        <v>20.228999999999999</v>
+      </c>
       <c r="G16">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>181.41</v>
       </c>
       <c r="I16">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>5.333333333333333</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="B17" t="s">
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17">
+        <v>9.7930000000000003E-2</v>
       </c>
       <c r="E17">
         <v>2</v>
       </c>
+      <c r="F17">
+        <v>23.741</v>
+      </c>
       <c r="G17">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>154.36000000000001</v>
       </c>
       <c r="I17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J17">
         <f t="shared" si="0"/>
-        <v>2.6666666666666665</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="B18" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18">
+        <v>0.10627</v>
       </c>
       <c r="E18">
         <v>3</v>
       </c>
+      <c r="F18">
+        <v>27.550999999999998</v>
+      </c>
       <c r="G18">
         <v>3</v>
       </c>
+      <c r="H18">
+        <v>151.22999999999999</v>
+      </c>
       <c r="I18">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J18">
         <f t="shared" si="0"/>
-        <v>4.333333333333333</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="4" t="s">
+        <v>2.3333333333333335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="3" customFormat="1">
+      <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="B20" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20">
+        <v>0.13664999999999999</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
+      <c r="F20">
+        <v>34.768000000000001</v>
+      </c>
       <c r="G20">
         <v>1</v>
       </c>
+      <c r="H20">
+        <v>256.97000000000003</v>
+      </c>
       <c r="I20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>2.3333333333333335</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="B21" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21">
+        <v>0.14968000000000001</v>
       </c>
       <c r="E21">
         <v>2</v>
       </c>
+      <c r="F21">
+        <v>46.81</v>
+      </c>
       <c r="G21">
         <v>2</v>
+      </c>
+      <c r="H21">
+        <v>420.83</v>
       </c>
       <c r="I21">
         <v>3</v>
@@ -1117,95 +1488,131 @@
     </row>
     <row r="22" spans="1:10">
       <c r="B22" t="s">
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22">
+        <v>0.16209000000000001</v>
       </c>
       <c r="E22">
         <v>3</v>
       </c>
+      <c r="F22">
+        <v>57.93</v>
+      </c>
       <c r="G22">
         <v>3</v>
       </c>
+      <c r="H22">
+        <v>391.59</v>
+      </c>
       <c r="I22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>3.3333333333333335</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="4" customFormat="1">
-      <c r="A23" s="4" t="s">
+        <v>2.6666666666666665</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="3" customFormat="1">
+      <c r="A23" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="B24" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24">
+        <v>0.20877000000000001</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
+      <c r="F24">
+        <v>120.78</v>
+      </c>
       <c r="G24">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>808.75</v>
       </c>
       <c r="I24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
-        <v>1.6666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="B25" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25">
+        <v>0.25957000000000002</v>
       </c>
       <c r="E25">
         <v>2</v>
       </c>
+      <c r="F25">
+        <v>183.81</v>
+      </c>
       <c r="G25">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>1491.5</v>
       </c>
       <c r="I25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J25">
         <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="B26" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>43</v>
+      <c r="C26" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="D26">
-        <v>8.9190000000000005E-2</v>
+        <v>0.28449000000000002</v>
       </c>
       <c r="E26">
         <v>3</v>
       </c>
       <c r="F26">
-        <v>14.928000000000001</v>
+        <v>208.49</v>
       </c>
       <c r="G26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H26">
-        <v>245.29</v>
+        <v>1723.8</v>
       </c>
       <c r="I26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>3.6666666666666665</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="4" customFormat="1">
-      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="3" customFormat="1">
+      <c r="A27" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1213,23 +1620,12 @@
       <c r="B28" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28">
-        <v>5.8840000000000003E-2</v>
-      </c>
+      <c r="C28" s="4"/>
       <c r="E28">
         <v>1</v>
       </c>
-      <c r="F28">
-        <v>8.8422000000000001</v>
-      </c>
       <c r="G28">
         <v>1</v>
-      </c>
-      <c r="H28">
-        <v>112.1</v>
       </c>
       <c r="I28">
         <v>1</v>
@@ -1241,137 +1637,133 @@
     </row>
     <row r="29" spans="1:10">
       <c r="B29" t="s">
-        <v>26</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C29" s="4"/>
       <c r="E29">
         <v>2</v>
       </c>
       <c r="G29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="B30" t="s">
-        <v>27</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C30" s="4"/>
       <c r="E30">
         <v>3</v>
       </c>
       <c r="G30">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I30">
         <v>4</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="4" customFormat="1">
-      <c r="A31" s="4" t="s">
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="3" customFormat="1">
+      <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="B32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D32">
-        <v>7.868E-2</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C32" s="4"/>
       <c r="E32">
         <v>1</v>
       </c>
-      <c r="F32">
-        <v>12.369</v>
-      </c>
       <c r="G32">
-        <v>1</v>
-      </c>
-      <c r="H32">
-        <v>66.311999999999998</v>
+        <v>2</v>
       </c>
       <c r="I32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="B33" t="s">
-        <v>26</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C33" s="4"/>
       <c r="E33">
         <v>2</v>
       </c>
       <c r="G33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>2.6666666666666665</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="B34" t="s">
-        <v>23</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C34" s="4"/>
       <c r="E34">
         <v>3</v>
       </c>
       <c r="G34">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="I34">
         <v>0</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" s="4" customFormat="1">
-      <c r="A35" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="3" customFormat="1">
+      <c r="A35" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="B36" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="E36">
         <v>1</v>
       </c>
       <c r="G36">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="B37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E37">
         <v>2</v>
@@ -1380,16 +1772,16 @@
         <v>2</v>
       </c>
       <c r="I37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>2.3333333333333335</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="B38" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E38">
         <v>3</v>
@@ -1398,51 +1790,42 @@
         <v>3</v>
       </c>
       <c r="I38">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
-        <v>2.6666666666666665</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" s="4" customFormat="1">
-      <c r="A39" s="4" t="s">
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="3" customFormat="1">
+      <c r="A39" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="B40" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40">
-        <v>9.4740000000000005E-2</v>
+        <v>29</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
-      <c r="F40">
-        <v>29.294</v>
-      </c>
       <c r="G40">
         <v>1</v>
       </c>
-      <c r="H40">
-        <v>165.81</v>
-      </c>
       <c r="I40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="B41" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E41">
         <v>2</v>
@@ -1451,16 +1834,16 @@
         <v>2</v>
       </c>
       <c r="I41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>1.6666666666666667</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="B42" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E42">
         <v>3</v>
@@ -1469,15 +1852,15 @@
         <v>3</v>
       </c>
       <c r="I42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>3.3333333333333335</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" s="4" customFormat="1">
-      <c r="A43" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="3" customFormat="1">
+      <c r="A43" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1485,6 +1868,9 @@
       <c r="B44" t="s">
         <v>29</v>
       </c>
+      <c r="C44" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="E44">
         <v>1</v>
       </c>
@@ -1492,17 +1878,18 @@
         <v>1</v>
       </c>
       <c r="I44">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="B45" t="s">
-        <v>26</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C45" s="4"/>
       <c r="E45">
         <v>2</v>
       </c>
@@ -1510,16 +1897,16 @@
         <v>2</v>
       </c>
       <c r="I45">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>7.333333333333333</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="B46" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E46">
         <v>3</v>
@@ -1528,15 +1915,15 @@
         <v>3</v>
       </c>
       <c r="I46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>2.3333333333333335</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" s="4" customFormat="1">
-      <c r="A47" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="3" customFormat="1">
+      <c r="A47" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1544,36 +1931,26 @@
       <c r="B48" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D48">
-        <v>6.3119999999999996E-2</v>
-      </c>
+      <c r="C48" s="4"/>
       <c r="E48">
         <v>1</v>
       </c>
-      <c r="F48">
-        <v>10.914999999999999</v>
-      </c>
       <c r="G48">
-        <v>22</v>
-      </c>
-      <c r="H48">
-        <v>125.97</v>
+        <v>1</v>
       </c>
       <c r="I48">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>9.6666666666666661</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="B49" t="s">
-        <v>31</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C49" s="4"/>
       <c r="E49">
         <v>2</v>
       </c>
@@ -1581,76 +1958,83 @@
         <v>2</v>
       </c>
       <c r="I49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2.6666666666666665</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="B50" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="E50">
         <v>3</v>
       </c>
       <c r="G50">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I50">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>3.6666666666666665</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" s="4" customFormat="1">
-      <c r="A51" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="3" customFormat="1">
+      <c r="A51" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="B52" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E52">
         <v>1</v>
       </c>
       <c r="G52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I52">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="B53" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="E53">
         <v>2</v>
       </c>
       <c r="G53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I53">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>3.6666666666666665</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="B54" t="s">
-        <v>29</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C54" s="4"/>
       <c r="E54">
         <v>3</v>
       </c>
@@ -1658,82 +2042,74 @@
         <v>3</v>
       </c>
       <c r="I54">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>2.6666666666666665</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" s="4" customFormat="1">
-      <c r="A55" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="3" customFormat="1">
+      <c r="A55" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="B56" t="s">
-        <v>30</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D56">
-        <v>9.2740000000000003E-2</v>
+        <v>29</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
-      <c r="F56">
-        <v>25.11</v>
-      </c>
       <c r="G56">
-        <v>1</v>
-      </c>
-      <c r="H56">
-        <v>159.25</v>
+        <v>2</v>
       </c>
       <c r="I56">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="B57" t="s">
-        <v>23</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C57" s="4"/>
       <c r="E57">
         <v>2</v>
       </c>
       <c r="G57">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="I57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J57">
         <f t="shared" si="0"/>
-        <v>16.333333333333332</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="B58" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E58">
         <v>3</v>
       </c>
       <c r="G58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I58">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>4.333333333333333</v>
+        <v>2.6666666666666665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>